<commit_message>
main page features files,step definitions and page objects commit
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/LMSTestData.xlsx
+++ b/src/test/resources/Exceldata/LMSTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auxilia/git/Team09_BDDCoders/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A4862D-70D3-334E-A5A4-3DC1B5FDD4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D9B59C-7FC8-9646-B1E6-80B2A1DD6570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>password</t>
   </si>
@@ -44,7 +44,37 @@
     <t>expected message</t>
   </si>
   <si>
-    <t>user</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>testuser</t>
+  </si>
+  <si>
+    <t>team@9%^</t>
+  </si>
+  <si>
+    <t>Please Check the Username/Password</t>
+  </si>
+  <si>
+    <t>Team9testuser</t>
+  </si>
+  <si>
+    <t>Please Check the Password</t>
+  </si>
+  <si>
+    <t>BddCoders@9</t>
+  </si>
+  <si>
+    <t>Please Check the Username</t>
+  </si>
+  <si>
+    <t>Please Enter the Username</t>
+  </si>
+  <si>
+    <t>Please Enter the Password</t>
+  </si>
+  <si>
+    <t>Please Enter the Username and Password</t>
   </si>
 </sst>
 </file>
@@ -413,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F830A691-D612-924F-8805-CA94148EB49D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -438,17 +466,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C2" s="2"/>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C3" s="2"/>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TestRunner and excel sheet update
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/LMSTestData.xlsx
+++ b/src/test/resources/Exceldata/LMSTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auxilia/git/Team09_BDDCoders/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C74AAB-59FC-CB4A-A9BC-CADF35F6A7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812975F-7E05-DF47-A4FF-6924DFC24FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" activeTab="1" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>password</t>
   </si>
@@ -76,13 +76,58 @@
   </si>
   <si>
     <t>Please Enter the Username and Password</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>linkdeinurl</t>
+  </si>
+  <si>
+    <t>usercomments</t>
+  </si>
+  <si>
+    <t>postgraduate</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>98675434</t>
+  </si>
+  <si>
+    <t>www.linkedin/ronj.com</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +150,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,15 +176,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,12 +586,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA22347-8582-0242-AAE4-F42DEC7AFF87}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{300FD22F-BF0E-274D-8750-F0EACD928512}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated config properties,configReader.java and LMSTestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/LMSTestData.xlsx
+++ b/src/test/resources/Exceldata/LMSTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auxilia/git/Team09_BDDCoders/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812975F-7E05-DF47-A4FF-6924DFC24FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5FF1A9-311E-B24E-B2EB-55FE515650CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" activeTab="1" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
+    <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" activeTab="2" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="AddNewUserDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="ManageClass" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>password</t>
   </si>
@@ -121,6 +122,114 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>NoOfClasses</t>
+  </si>
+  <si>
+    <t>ValidBatchId</t>
+  </si>
+  <si>
+    <t>InvalidBatchId</t>
+  </si>
+  <si>
+    <t>ValidClassNo</t>
+  </si>
+  <si>
+    <t>InvalidClassNo</t>
+  </si>
+  <si>
+    <t>ValidClassDate</t>
+  </si>
+  <si>
+    <t>InvalidClassDate</t>
+  </si>
+  <si>
+    <t>ValidClassTopic</t>
+  </si>
+  <si>
+    <t>InvalidClassTopic</t>
+  </si>
+  <si>
+    <t>ValidStaffId</t>
+  </si>
+  <si>
+    <t>InvalidStaffId</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Recordings</t>
+  </si>
+  <si>
+    <t>SudhaBatch</t>
+  </si>
+  <si>
+    <t>SDET+JAVA</t>
+  </si>
+  <si>
+    <t>QA-Automation</t>
+  </si>
+  <si>
+    <t>"14"</t>
+  </si>
+  <si>
+    <t>"1343"</t>
+  </si>
+  <si>
+    <t>"327654"</t>
+  </si>
+  <si>
+    <t>"23"</t>
+  </si>
+  <si>
+    <t>"6897"</t>
+  </si>
+  <si>
+    <t>"12/22/2023"</t>
+  </si>
+  <si>
+    <t>"9/22/2024"</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>"U78"</t>
+  </si>
+  <si>
+    <t>"U90000"</t>
+  </si>
+  <si>
+    <t>Advanced Python</t>
+  </si>
+  <si>
+    <t>SelfLearning</t>
+  </si>
+  <si>
+    <t>python Notes</t>
+  </si>
+  <si>
+    <t>c:\\Recordings</t>
   </si>
 </sst>
 </file>
@@ -180,12 +289,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA22347-8582-0242-AAE4-F42DEC7AFF87}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -652,4 +764,131 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEF89CF-15BF-C943-A141-1F8647FC1977}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #5 from sudha-singh/Auxilia"
This reverts commit cb467fae70b999ad63feea634db343d206ccf05f, reversing
changes made to 6f18cee898f4313f9fcc14e770b3f8f650d089cb.
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/LMSTestData.xlsx
+++ b/src/test/resources/Exceldata/LMSTestData.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auxilia/git/Team09_BDDCoders/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5FF1A9-311E-B24E-B2EB-55FE515650CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812975F-7E05-DF47-A4FF-6924DFC24FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" activeTab="2" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
+    <workbookView xWindow="7640" yWindow="500" windowWidth="21160" windowHeight="16300" activeTab="1" xr2:uid="{18938CFE-15B3-A64D-A13E-D57D8BC40BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="AddNewUserDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="ManageClass" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>password</t>
   </si>
@@ -122,114 +121,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>BatchName</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ProgramName</t>
-  </si>
-  <si>
-    <t>NoOfClasses</t>
-  </si>
-  <si>
-    <t>ValidBatchId</t>
-  </si>
-  <si>
-    <t>InvalidBatchId</t>
-  </si>
-  <si>
-    <t>ValidClassNo</t>
-  </si>
-  <si>
-    <t>InvalidClassNo</t>
-  </si>
-  <si>
-    <t>ValidClassDate</t>
-  </si>
-  <si>
-    <t>InvalidClassDate</t>
-  </si>
-  <si>
-    <t>ValidClassTopic</t>
-  </si>
-  <si>
-    <t>InvalidClassTopic</t>
-  </si>
-  <si>
-    <t>ValidStaffId</t>
-  </si>
-  <si>
-    <t>InvalidStaffId</t>
-  </si>
-  <si>
-    <t>ClassDescription</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Recordings</t>
-  </si>
-  <si>
-    <t>SudhaBatch</t>
-  </si>
-  <si>
-    <t>SDET+JAVA</t>
-  </si>
-  <si>
-    <t>QA-Automation</t>
-  </si>
-  <si>
-    <t>"14"</t>
-  </si>
-  <si>
-    <t>"1343"</t>
-  </si>
-  <si>
-    <t>"327654"</t>
-  </si>
-  <si>
-    <t>"23"</t>
-  </si>
-  <si>
-    <t>"6897"</t>
-  </si>
-  <si>
-    <t>"12/22/2023"</t>
-  </si>
-  <si>
-    <t>"9/22/2024"</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>"U78"</t>
-  </si>
-  <si>
-    <t>"U90000"</t>
-  </si>
-  <si>
-    <t>Advanced Python</t>
-  </si>
-  <si>
-    <t>SelfLearning</t>
-  </si>
-  <si>
-    <t>python Notes</t>
-  </si>
-  <si>
-    <t>c:\\Recordings</t>
   </si>
 </sst>
 </file>
@@ -289,15 +180,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA22347-8582-0242-AAE4-F42DEC7AFF87}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -764,131 +652,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEF89CF-15BF-C943-A141-1F8647FC1977}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>